<commit_message>
latest changes for ui
</commit_message>
<xml_diff>
--- a/src/assets/excel/Book1.xlsx
+++ b/src/assets/excel/Book1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
   <si>
     <t>201A</t>
   </si>
@@ -112,16 +112,28 @@
     <t>Vedant Kangulwar</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>RollNO</t>
-  </si>
-  <si>
-    <t>FullName</t>
-  </si>
-  <si>
     <t>image</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>FName</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Address</t>
   </si>
 </sst>
 </file>
@@ -215,25 +227,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -242,6 +251,619 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1188976</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>817501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="stud1.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4486276" y="285751"/>
+          <a:ext cx="1008000" cy="731775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1188976</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>817501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7" descr="stud1.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4486276" y="285751"/>
+          <a:ext cx="1008000" cy="731775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1188976</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>817501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8" descr="stud1.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4486276" y="285751"/>
+          <a:ext cx="1008000" cy="731775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1188976</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>817501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9" descr="stud1.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4486276" y="285751"/>
+          <a:ext cx="1008000" cy="731775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1188976</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>817501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10" descr="stud1.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4486276" y="285751"/>
+          <a:ext cx="1008000" cy="731775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1188976</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>817501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11" descr="stud1.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4486276" y="285751"/>
+          <a:ext cx="1008000" cy="731775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1188976</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>817501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12" descr="stud1.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4486276" y="285751"/>
+          <a:ext cx="1008000" cy="731775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1188976</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>817501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13" descr="stud1.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4486276" y="285751"/>
+          <a:ext cx="1008000" cy="731775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1188976</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>817501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14" descr="stud1.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4486276" y="285751"/>
+          <a:ext cx="1008000" cy="731775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1188976</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>817501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15" descr="stud1.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4486276" y="285751"/>
+          <a:ext cx="1008000" cy="731775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1188976</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>817501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16" descr="stud1.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4486276" y="285751"/>
+          <a:ext cx="1008000" cy="731775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1188976</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>817501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17" descr="stud1.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4486276" y="285751"/>
+          <a:ext cx="1008000" cy="731775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1188976</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>817501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18" descr="stud1.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4486276" y="285751"/>
+          <a:ext cx="1008000" cy="731775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1188976</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>817501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19" descr="stud1.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4486276" y="285751"/>
+          <a:ext cx="1008000" cy="731775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1188976</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>817501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20" descr="stud1.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4486276" y="285751"/>
+          <a:ext cx="1008000" cy="731775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1188976</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>817501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21" descr="stud1.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4486276" y="285751"/>
+          <a:ext cx="1008000" cy="731775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -529,210 +1151,368 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1">
       <c r="A1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="68.25" customHeight="1" thickBot="1">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5">
+        <v>44593</v>
+      </c>
+      <c r="E2">
+        <v>7589874589</v>
+      </c>
+      <c r="F2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="4">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="D3" s="5">
+        <v>44594</v>
+      </c>
+      <c r="E3">
+        <v>7589874589</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="D4" s="5">
+        <v>44595</v>
+      </c>
+      <c r="E4">
+        <v>7589874589</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="D5" s="5">
+        <v>44596</v>
+      </c>
+      <c r="E5">
+        <v>7589874589</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="4">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="D6" s="5">
+        <v>44597</v>
+      </c>
+      <c r="E6">
+        <v>7589874589</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="4">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="D7" s="5">
+        <v>44598</v>
+      </c>
+      <c r="E7">
+        <v>7589874589</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5" t="s">
+      <c r="D8" s="5">
+        <v>44599</v>
+      </c>
+      <c r="E8">
+        <v>7589874589</v>
+      </c>
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="D9" s="5">
+        <v>44600</v>
+      </c>
+      <c r="E9">
+        <v>7589874589</v>
+      </c>
+      <c r="F9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="4">
-        <v>10</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="D10" s="5">
+        <v>44601</v>
+      </c>
+      <c r="E10">
+        <v>7589874589</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="D11" s="5">
+        <v>44602</v>
+      </c>
+      <c r="E11">
+        <v>7589874589</v>
+      </c>
+      <c r="F11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
+      <c r="D12" s="5">
+        <v>44603</v>
+      </c>
+      <c r="E12">
+        <v>7589874589</v>
+      </c>
+      <c r="F12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="4">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="s">
+      <c r="D13" s="5">
+        <v>44604</v>
+      </c>
+      <c r="E13">
+        <v>7589874589</v>
+      </c>
+      <c r="F13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="4">
-        <v>14</v>
-      </c>
-      <c r="B15" s="5" t="s">
+      <c r="D14" s="5">
+        <v>44605</v>
+      </c>
+      <c r="E14">
+        <v>7589874589</v>
+      </c>
+      <c r="F14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="4">
-        <v>15</v>
-      </c>
-      <c r="B16" s="5" t="s">
+      <c r="D15" s="5">
+        <v>44606</v>
+      </c>
+      <c r="E15">
+        <v>7589874589</v>
+      </c>
+      <c r="F15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="4">
-        <v>16</v>
-      </c>
-      <c r="B17" s="5" t="s">
+      <c r="D16" s="5">
+        <v>44607</v>
+      </c>
+      <c r="E16">
+        <v>7589874589</v>
+      </c>
+      <c r="F16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>31</v>
+      </c>
+      <c r="D17" s="5">
+        <v>44608</v>
+      </c>
+      <c r="E17">
+        <v>7589874589</v>
+      </c>
+      <c r="F17" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>